<commit_message>
--fix on setCellData. Now could create a new cell
</commit_message>
<xml_diff>
--- a/src/test/java/west/com/OxygenThree/DataDrivenDataSet/OnlineStore_DataDriven_Login.xlsx
+++ b/src/test/java/west/com/OxygenThree/DataDrivenDataSet/OnlineStore_DataDriven_Login.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Function Name</t>
   </si>
@@ -44,12 +44,19 @@
   <si>
     <t>testuser_12345678|Test@123</t>
   </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,14 +68,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -91,19 +90,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -191,7 +187,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -226,7 +221,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -402,21 +396,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="29.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -433,7 +427,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -443,8 +437,21 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="F8" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -457,24 +464,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
--implement getRowContains and test it
</commit_message>
<xml_diff>
--- a/src/test/java/west/com/OxygenThree/DataDrivenDataSet/OnlineStore_DataDriven_Login.xlsx
+++ b/src/test/java/west/com/OxygenThree/DataDrivenDataSet/OnlineStore_DataDriven_Login.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>Function Name</t>
   </si>
@@ -45,17 +45,19 @@
     <t>testuser_12345678|Test@123</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>test2</t>
+    <t>RunTestCase_ICSLogin</t>
+  </si>
+  <si>
+    <t>admin|Admin</t>
+  </si>
+  <si>
+    <t>testuser_1234|Test@123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -397,17 +399,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="29.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -440,23 +442,39 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="6">
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="F8" t="s">
-        <v>10</v>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>